<commit_message>
FR-6041: fix review issues.
</commit_message>
<xml_diff>
--- a/app/resources/users_import_template_en.xlsx
+++ b/app/resources/users_import_template_en.xlsx
@@ -167,7 +167,7 @@
     <t>Device limit</t>
   </si>
   <si>
-    <t>navixy@navixy.com</t>
+    <t>email@example.com</t>
   </si>
   <si>
     <t>e$0M#1Cr</t>
@@ -250,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -263,13 +263,14 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -652,13 +653,13 @@
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>1.0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>2.0</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -668,51 +669,51 @@
         <v>28</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="5">
-        <f>79999999999</f>
-        <v>79999999999</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="6">
+        <f>17189164558</f>
+        <v>17189164558</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>11230.0</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="6" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="4">
         <v>11230.0</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="4">
         <v>5.0</v>
       </c>
-      <c r="X2" s="7">
+      <c r="X2" s="8">
         <v>55153.0</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="5">
         <v>10.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FR-6871: upload new xlsx files
</commit_message>
<xml_diff>
--- a/app/resources/users_import_template_en.xlsx
+++ b/app/resources/users_import_template_en.xlsx
@@ -1,88 +1,187 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C1">
-      <text>
-        <t xml:space="preserve">1-  if user activated (allowed to login);
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>1-  if user activated (allowed to login);
 0 - if the user blocked (not allowed to login)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D1">
-      <text>
-        <t xml:space="preserve">1- individual, 
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">1- individual, 
 2- legal entity,
 3- sole trader
 </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="J1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="K1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="L1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="M1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="N1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="O1">
-      <text>
-        <t xml:space="preserve">required for legal entity</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="R1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="S1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="T1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="U1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="V1">
-      <text>
-        <t xml:space="preserve">required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>required for legal entity and sole trader</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -90,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Email address*</t>
   </si>
@@ -167,9 +266,6 @@
     <t>Device limit</t>
   </si>
   <si>
-    <t>email@example.com</t>
-  </si>
-  <si>
     <t>e$0M#1Cr</t>
   </si>
   <si>
@@ -189,36 +285,59 @@
   </si>
   <si>
     <t>123 Westminster Avenue APT A2</t>
+  </si>
+  <si>
+    <t>Legal Name</t>
+  </si>
+  <si>
+    <t>individual@example.com</t>
+  </si>
+  <si>
+    <t>legal@example.com</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.MM.yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
-      <color rgb="FF000000"/>
-    </font>
-    <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -227,11 +346,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -245,127 +370,135 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD9D9D9"/>
           <bgColor rgb="FFD9D9D9"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Лист1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Лист1-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Y2" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:Y3">
   <tableColumns count="25">
-    <tableColumn name="Email address*" id="1"/>
-    <tableColumn name="Password*" id="2"/>
-    <tableColumn name="Status*" id="3"/>
-    <tableColumn name="Legal status*" id="4"/>
-    <tableColumn name="Surname*" id="5"/>
-    <tableColumn name="Name*" id="6"/>
-    <tableColumn name="Middle name" id="7"/>
-    <tableColumn name="Phone number" id="8"/>
-    <tableColumn name="Сomment" id="9"/>
-    <tableColumn name="Country" id="10"/>
-    <tableColumn name="Region" id="11"/>
-    <tableColumn name="City" id="12"/>
-    <tableColumn name="Street, address" id="13"/>
-    <tableColumn name="Zip code" id="14"/>
-    <tableColumn name="Legal name" id="15"/>
-    <tableColumn name="Tax number" id="16"/>
-    <tableColumn name="IEC" id="17"/>
-    <tableColumn name="Registration country" id="18"/>
-    <tableColumn name="Registration region" id="19"/>
-    <tableColumn name="Registration city        " id="20"/>
-    <tableColumn name="Registration address" id="21"/>
-    <tableColumn name="Registration zip code" id="22"/>
-    <tableColumn name="Discount" id="23"/>
-    <tableColumn name="End date of discount" id="24"/>
-    <tableColumn name="Device limit" id="25"/>
+    <tableColumn id="1" name="Email address*" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="2" name="Password*"/>
+    <tableColumn id="3" name="Status*"/>
+    <tableColumn id="4" name="Legal status*"/>
+    <tableColumn id="5" name="Surname*"/>
+    <tableColumn id="6" name="Name*"/>
+    <tableColumn id="7" name="Middle name"/>
+    <tableColumn id="8" name="Phone number"/>
+    <tableColumn id="9" name="Сomment"/>
+    <tableColumn id="10" name="Country"/>
+    <tableColumn id="11" name="Region"/>
+    <tableColumn id="12" name="City"/>
+    <tableColumn id="13" name="Street, address"/>
+    <tableColumn id="14" name="Zip code"/>
+    <tableColumn id="15" name="Legal name"/>
+    <tableColumn id="16" name="Tax number"/>
+    <tableColumn id="17" name="IEC"/>
+    <tableColumn id="18" name="Registration country"/>
+    <tableColumn id="19" name="Registration region"/>
+    <tableColumn id="20" name="Registration city        "/>
+    <tableColumn id="21" name="Registration address"/>
+    <tableColumn id="22" name="Registration zip code"/>
+    <tableColumn id="23" name="Discount"/>
+    <tableColumn id="24" name="End date of discount"/>
+    <tableColumn id="25" name="Device limit"/>
   </tableColumns>
-  <tableStyleInfo name="Лист1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Лист1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -555,24 +688,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.86"/>
-    <col customWidth="1" min="21" max="21" width="15.14"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="21" max="21" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:25" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,24 +785,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:25" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="6">
@@ -675,53 +811,98 @@
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4">
+        <v>11230</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="4">
-        <v>11230.0</v>
-      </c>
-      <c r="O2" s="4"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="V2" s="4">
-        <v>11230.0</v>
+        <v>11230</v>
       </c>
       <c r="W2" s="4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="X2" s="8">
-        <v>55153.0</v>
+        <v>55153</v>
       </c>
       <c r="Y2" s="5">
-        <v>10.0</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="11"/>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>